<commit_message>
Dodawanie wykresów i poprawionych danych. Trzeba poprawić Tytuły wykresów.
</commit_message>
<xml_diff>
--- a/dane_panelowe.xlsx
+++ b/dane_panelowe.xlsx
@@ -5,17 +5,30 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michalksiazek/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michalksiazek/Documents/ekonometria/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5600063C-C753-4F4B-8F18-2FFB909D9CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4778D6-D8E9-3F4A-B124-1AA57E36147C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -143,7 +156,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.##########"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,13 +175,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F6F6"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -195,11 +221,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -507,7 +547,7 @@
   <dimension ref="A1:L325"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -589,8 +629,8 @@
       <c r="I2">
         <v>58264.78</v>
       </c>
-      <c r="J2">
-        <v>58264.78</v>
+      <c r="J2" s="2">
+        <v>1.04</v>
       </c>
       <c r="K2">
         <v>2</v>
@@ -627,8 +667,8 @@
       <c r="I3">
         <v>7596.11</v>
       </c>
-      <c r="J3">
-        <v>7596.11</v>
+      <c r="J3" s="4">
+        <v>0.56000000000000005</v>
       </c>
       <c r="K3">
         <v>8.9</v>
@@ -665,8 +705,8 @@
       <c r="I4">
         <v>19542.97</v>
       </c>
-      <c r="J4">
-        <v>19542.97</v>
+      <c r="J4" s="2">
+        <v>0.75</v>
       </c>
       <c r="K4">
         <v>-0.2</v>
@@ -703,8 +743,8 @@
       <c r="I5">
         <v>71088.850000000006</v>
       </c>
-      <c r="J5">
-        <v>71088.850000000006</v>
+      <c r="J5" s="4">
+        <v>1.1299999999999999</v>
       </c>
       <c r="K5">
         <v>0.3</v>
@@ -741,8 +781,8 @@
       <c r="I6">
         <v>59427.97</v>
       </c>
-      <c r="J6">
-        <v>59427.97</v>
+      <c r="J6" s="2">
+        <v>1.1499999999999999</v>
       </c>
       <c r="K6">
         <v>2.2999999999999998</v>
@@ -779,8 +819,8 @@
       <c r="I7">
         <v>19714.59</v>
       </c>
-      <c r="J7">
-        <v>19714.59</v>
+      <c r="J7" s="4">
+        <v>0.9</v>
       </c>
       <c r="K7">
         <v>4.9000000000000004</v>
@@ -817,8 +857,8 @@
       <c r="I8">
         <v>66182.559999999998</v>
       </c>
-      <c r="J8">
-        <v>66182.559999999998</v>
+      <c r="J8" s="2">
+        <v>1.36</v>
       </c>
       <c r="K8">
         <v>-0.2</v>
@@ -855,8 +895,8 @@
       <c r="I9">
         <v>33939.78</v>
       </c>
-      <c r="J9">
-        <v>33939.78</v>
+      <c r="J9" s="4">
+        <v>0.78</v>
       </c>
       <c r="K9">
         <v>-6.3</v>
@@ -893,8 +933,8 @@
       <c r="I10">
         <v>41083.089999999997</v>
       </c>
-      <c r="J10">
-        <v>41083.089999999997</v>
+      <c r="J10" s="2">
+        <v>0.9</v>
       </c>
       <c r="K10">
         <v>-0.4</v>
@@ -931,8 +971,8 @@
       <c r="I11">
         <v>55466.16</v>
       </c>
-      <c r="J11">
-        <v>55466.16</v>
+      <c r="J11" s="4">
+        <v>0.97</v>
       </c>
       <c r="K11">
         <v>1.3</v>
@@ -969,8 +1009,8 @@
       <c r="I12">
         <v>16779.900000000001</v>
       </c>
-      <c r="J12">
-        <v>16779.900000000001</v>
+      <c r="J12" s="2">
+        <v>0.71</v>
       </c>
       <c r="K12">
         <v>-3.1</v>
@@ -1007,8 +1047,8 @@
       <c r="I13">
         <v>43358.61</v>
       </c>
-      <c r="J13">
-        <v>43358.61</v>
+      <c r="J13" s="4">
+        <v>0.97</v>
       </c>
       <c r="K13">
         <v>0.8</v>
@@ -1042,8 +1082,8 @@
       <c r="H14">
         <v>93.8</v>
       </c>
-      <c r="J14">
-        <v>38952.93</v>
+      <c r="J14" s="2">
+        <v>1.04</v>
       </c>
       <c r="K14">
         <v>-4.0999999999999996</v>
@@ -1080,8 +1120,8 @@
       <c r="I15">
         <v>12441.56</v>
       </c>
-      <c r="J15">
-        <v>12441.56</v>
+      <c r="J15" s="4">
+        <v>0.83</v>
       </c>
       <c r="K15">
         <v>5.9</v>
@@ -1118,8 +1158,8 @@
       <c r="I16">
         <v>12066.17</v>
       </c>
-      <c r="J16">
-        <v>12066.17</v>
+      <c r="J16" s="2">
+        <v>0.84</v>
       </c>
       <c r="K16">
         <v>2.6</v>
@@ -1156,8 +1196,8 @@
       <c r="I17">
         <v>84962.73</v>
       </c>
-      <c r="J17">
-        <v>84962.73</v>
+      <c r="J17" s="4">
+        <v>1.28</v>
       </c>
       <c r="K17">
         <v>1.8</v>
@@ -1194,8 +1234,8 @@
       <c r="I18">
         <v>14833.81</v>
       </c>
-      <c r="J18">
-        <v>14833.81</v>
+      <c r="J18" s="2">
+        <v>0.61</v>
       </c>
       <c r="K18">
         <v>-0.7</v>
@@ -1232,8 +1272,8 @@
       <c r="I19">
         <v>34228.720000000001</v>
       </c>
-      <c r="J19">
-        <v>34228.720000000001</v>
+      <c r="J19" s="4">
+        <v>1.08</v>
       </c>
       <c r="K19">
         <v>0.7</v>
@@ -1270,8 +1310,8 @@
       <c r="I20">
         <v>69978.34</v>
       </c>
-      <c r="J20">
-        <v>69978.34</v>
+      <c r="J20" s="2">
+        <v>1.22</v>
       </c>
       <c r="K20">
         <v>0.7</v>
@@ -1308,8 +1348,8 @@
       <c r="I21">
         <v>60166.04</v>
       </c>
-      <c r="J21">
-        <v>60166.04</v>
+      <c r="J21" s="4">
+        <v>0.96</v>
       </c>
       <c r="K21">
         <v>2.5</v>
@@ -1346,8 +1386,8 @@
       <c r="I22">
         <v>15462.31</v>
       </c>
-      <c r="J22">
-        <v>15462.31</v>
+      <c r="J22" s="2">
+        <v>0.68</v>
       </c>
       <c r="K22">
         <v>0.9</v>
@@ -1384,8 +1424,8 @@
       <c r="I23">
         <v>24225.61</v>
       </c>
-      <c r="J23">
-        <v>24225.61</v>
+      <c r="J23" s="4">
+        <v>0.82</v>
       </c>
       <c r="K23">
         <v>1.3</v>
@@ -1422,8 +1462,8 @@
       <c r="I24">
         <v>8945.8799999999992</v>
       </c>
-      <c r="J24">
-        <v>8945.8799999999992</v>
+      <c r="J24" s="2">
+        <v>0.56999999999999995</v>
       </c>
       <c r="K24">
         <v>3.7</v>
@@ -1460,8 +1500,8 @@
       <c r="I25">
         <v>25855.18</v>
       </c>
-      <c r="J25">
-        <v>25855.18</v>
+      <c r="J25" s="4">
+        <v>0.85</v>
       </c>
       <c r="K25">
         <v>0.1</v>
@@ -1498,8 +1538,8 @@
       <c r="I26">
         <v>16936.849999999999</v>
       </c>
-      <c r="J26">
-        <v>16936.849999999999</v>
+      <c r="J26" s="2">
+        <v>0.63</v>
       </c>
       <c r="K26">
         <v>1.1000000000000001</v>
@@ -1536,8 +1576,8 @@
       <c r="I27">
         <v>61940.14</v>
       </c>
-      <c r="J27">
-        <v>61940.14</v>
+      <c r="J27" s="4">
+        <v>1.1499999999999999</v>
       </c>
       <c r="K27">
         <v>1.4</v>
@@ -1574,8 +1614,8 @@
       <c r="I28">
         <v>72067.73</v>
       </c>
-      <c r="J28">
-        <v>72067.73</v>
+      <c r="J28" s="2">
+        <v>1.18</v>
       </c>
       <c r="K28">
         <v>1.6</v>
@@ -1612,8 +1652,8 @@
       <c r="I29">
         <v>58619.59</v>
       </c>
-      <c r="J29">
-        <v>58619.59</v>
+      <c r="J29" s="2">
+        <v>1.07</v>
       </c>
       <c r="K29">
         <v>-0.4</v>
@@ -1650,8 +1690,8 @@
       <c r="I30">
         <v>8067.46</v>
       </c>
-      <c r="J30">
-        <v>8067.46</v>
+      <c r="J30" s="4">
+        <v>0.57999999999999996</v>
       </c>
       <c r="K30">
         <v>5</v>
@@ -1688,8 +1728,8 @@
       <c r="I31">
         <v>18895.14</v>
       </c>
-      <c r="J31">
-        <v>18895.14</v>
+      <c r="J31" s="2">
+        <v>0.76</v>
       </c>
       <c r="K31">
         <v>1.2</v>
@@ -1726,8 +1766,8 @@
       <c r="I32">
         <v>72084.58</v>
       </c>
-      <c r="J32">
-        <v>72084.58</v>
+      <c r="J32" s="4">
+        <v>1.17</v>
       </c>
       <c r="K32">
         <v>0.8</v>
@@ -1764,8 +1804,8 @@
       <c r="I33">
         <v>60720.55</v>
       </c>
-      <c r="J33">
-        <v>60720.55</v>
+      <c r="J33" s="2">
+        <v>1.1299999999999999</v>
       </c>
       <c r="K33">
         <v>1.4</v>
@@ -1802,8 +1842,8 @@
       <c r="I34">
         <v>20653.099999999999</v>
       </c>
-      <c r="J34">
-        <v>20653.099999999999</v>
+      <c r="J34" s="4">
+        <v>0.92</v>
       </c>
       <c r="K34">
         <v>3.8</v>
@@ -1840,8 +1880,8 @@
       <c r="I35">
         <v>66494.77</v>
       </c>
-      <c r="J35">
-        <v>66494.77</v>
+      <c r="J35" s="2">
+        <v>1.41</v>
       </c>
       <c r="K35">
         <v>-5.0999999999999996</v>
@@ -1878,8 +1918,8 @@
       <c r="I36">
         <v>34510.379999999997</v>
       </c>
-      <c r="J36">
-        <v>34510.379999999997</v>
+      <c r="J36" s="4">
+        <v>0.77</v>
       </c>
       <c r="K36">
         <v>-2.5</v>
@@ -1916,8 +1956,8 @@
       <c r="I37">
         <v>41298.25</v>
       </c>
-      <c r="J37">
-        <v>41298.25</v>
+      <c r="J37" s="2">
+        <v>0.92</v>
       </c>
       <c r="K37">
         <v>-0.1</v>
@@ -1954,8 +1994,8 @@
       <c r="I38">
         <v>56178.45</v>
       </c>
-      <c r="J38">
-        <v>56178.45</v>
+      <c r="J38" s="4">
+        <v>0.98</v>
       </c>
       <c r="K38">
         <v>0.7</v>
@@ -1992,8 +2032,8 @@
       <c r="I39">
         <v>16853.599999999999</v>
       </c>
-      <c r="J39">
-        <v>16853.599999999999</v>
+      <c r="J39" s="2">
+        <v>0.72</v>
       </c>
       <c r="K39">
         <v>-1.7</v>
@@ -2030,8 +2070,8 @@
       <c r="I40">
         <v>43897.95</v>
       </c>
-      <c r="J40">
-        <v>43897.95</v>
+      <c r="J40" s="5">
+        <v>1</v>
       </c>
       <c r="K40">
         <v>0.2</v>
@@ -2068,8 +2108,8 @@
       <c r="I41">
         <v>38952.93</v>
       </c>
-      <c r="J41">
-        <v>38952.93</v>
+      <c r="J41" s="2">
+        <v>1.07</v>
       </c>
       <c r="K41">
         <v>-3.5</v>
@@ -2106,8 +2146,8 @@
       <c r="I42">
         <v>13752.2</v>
       </c>
-      <c r="J42">
-        <v>13752.2</v>
+      <c r="J42" s="4">
+        <v>0.85</v>
       </c>
       <c r="K42">
         <v>4.5999999999999996</v>
@@ -2144,8 +2184,8 @@
       <c r="I43">
         <v>12777.47</v>
       </c>
-      <c r="J43">
-        <v>12777.47</v>
+      <c r="J43" s="2">
+        <v>0.82</v>
       </c>
       <c r="K43">
         <v>2.7</v>
@@ -2182,8 +2222,8 @@
       <c r="I44">
         <v>86265.67</v>
       </c>
-      <c r="J44">
-        <v>86265.67</v>
+      <c r="J44" s="4">
+        <v>1.27</v>
       </c>
       <c r="K44">
         <v>2</v>
@@ -2220,8 +2260,8 @@
       <c r="I45">
         <v>14768.25</v>
       </c>
-      <c r="J45">
-        <v>14768.25</v>
+      <c r="J45" s="2">
+        <v>0.63</v>
       </c>
       <c r="K45">
         <v>0.4</v>
@@ -2258,8 +2298,8 @@
       <c r="I46">
         <v>33650</v>
       </c>
-      <c r="J46">
-        <v>33650</v>
+      <c r="J46" s="4">
+        <v>1.1100000000000001</v>
       </c>
       <c r="K46">
         <v>0.2</v>
@@ -2296,8 +2336,8 @@
       <c r="I47">
         <v>71442.7</v>
       </c>
-      <c r="J47">
-        <v>71442.7</v>
+      <c r="J47" s="2">
+        <v>1.22</v>
       </c>
       <c r="K47">
         <v>0.1</v>
@@ -2334,8 +2374,8 @@
       <c r="I48">
         <v>61122.86</v>
       </c>
-      <c r="J48">
-        <v>61122.86</v>
+      <c r="J48" s="4">
+        <v>0.96</v>
       </c>
       <c r="K48">
         <v>1.7</v>
@@ -2372,8 +2412,8 @@
       <c r="I49">
         <v>16513.87</v>
       </c>
-      <c r="J49">
-        <v>16513.87</v>
+      <c r="J49" s="2">
+        <v>0.7</v>
       </c>
       <c r="K49">
         <v>0.1</v>
@@ -2410,8 +2450,8 @@
       <c r="I50">
         <v>24087.78</v>
       </c>
-      <c r="J50">
-        <v>24087.78</v>
+      <c r="J50" s="4">
+        <v>0.85</v>
       </c>
       <c r="K50">
         <v>-1.2</v>
@@ -2448,8 +2488,8 @@
       <c r="I51">
         <v>9477.15</v>
       </c>
-      <c r="J51">
-        <v>9477.15</v>
+      <c r="J51" s="2">
+        <v>0.57999999999999996</v>
       </c>
       <c r="K51">
         <v>3.2</v>
@@ -2486,8 +2526,8 @@
       <c r="I52">
         <v>26191.52</v>
       </c>
-      <c r="J52">
-        <v>26191.52</v>
+      <c r="J52" s="4">
+        <v>0.86</v>
       </c>
       <c r="K52">
         <v>-0.8</v>
@@ -2524,8 +2564,8 @@
       <c r="I53">
         <v>17578.97</v>
       </c>
-      <c r="J53">
-        <v>17578.97</v>
+      <c r="J53" s="2">
+        <v>0.64</v>
       </c>
       <c r="K53">
         <v>0.5</v>
@@ -2562,8 +2602,8 @@
       <c r="I54">
         <v>61914.6</v>
       </c>
-      <c r="J54">
-        <v>61914.6</v>
+      <c r="J54" s="4">
+        <v>1.1499999999999999</v>
       </c>
       <c r="K54">
         <v>0.9</v>
@@ -2600,8 +2640,8 @@
       <c r="I55">
         <v>70814.09</v>
       </c>
-      <c r="J55">
-        <v>70814.09</v>
+      <c r="J55" s="2">
+        <v>1.19</v>
       </c>
       <c r="K55">
         <v>1.5</v>
@@ -2638,8 +2678,8 @@
       <c r="I56">
         <v>58953.77</v>
       </c>
-      <c r="J56">
-        <v>58953.77</v>
+      <c r="J56" s="2">
+        <v>1.06</v>
       </c>
       <c r="K56">
         <v>-0.6</v>
@@ -2676,8 +2716,8 @@
       <c r="I57">
         <v>8678.2900000000009</v>
       </c>
-      <c r="J57">
-        <v>8678.2900000000009</v>
+      <c r="J57" s="4">
+        <v>0.62</v>
       </c>
       <c r="K57">
         <v>2.6</v>
@@ -2714,8 +2754,8 @@
       <c r="I58">
         <v>19641.88</v>
       </c>
-      <c r="J58">
-        <v>19641.88</v>
+      <c r="J58" s="2">
+        <v>0.78</v>
       </c>
       <c r="K58">
         <v>-0.2</v>
@@ -2752,8 +2792,8 @@
       <c r="I59">
         <v>72810.09</v>
       </c>
-      <c r="J59">
-        <v>72810.09</v>
+      <c r="J59" s="4">
+        <v>1.18</v>
       </c>
       <c r="K59">
         <v>1.4</v>
@@ -2790,8 +2830,8 @@
       <c r="I60">
         <v>62112.47</v>
       </c>
-      <c r="J60">
-        <v>62112.47</v>
+      <c r="J60" s="2">
+        <v>1.1000000000000001</v>
       </c>
       <c r="K60">
         <v>1.9</v>
@@ -2828,8 +2868,8 @@
       <c r="I61">
         <v>22726.43</v>
       </c>
-      <c r="J61">
-        <v>22726.43</v>
+      <c r="J61" s="4">
+        <v>0.95</v>
       </c>
       <c r="K61">
         <v>4.2</v>
@@ -2866,8 +2906,8 @@
       <c r="I62">
         <v>67929.03</v>
       </c>
-      <c r="J62">
-        <v>67929.03</v>
+      <c r="J62" s="2">
+        <v>1.4</v>
       </c>
       <c r="K62">
         <v>-15</v>
@@ -2904,8 +2944,8 @@
       <c r="I63">
         <v>33887.46</v>
       </c>
-      <c r="J63">
-        <v>33887.46</v>
+      <c r="J63" s="4">
+        <v>0.78</v>
       </c>
       <c r="K63">
         <v>-4</v>
@@ -2942,8 +2982,8 @@
       <c r="I64">
         <v>42658.77</v>
       </c>
-      <c r="J64">
-        <v>42658.77</v>
+      <c r="J64" s="2">
+        <v>0.94</v>
       </c>
       <c r="K64">
         <v>-0.1</v>
@@ -2980,8 +3020,8 @@
       <c r="I65">
         <v>56979.66</v>
       </c>
-      <c r="J65">
-        <v>56979.66</v>
+      <c r="J65" s="4">
+        <v>0.98</v>
       </c>
       <c r="K65">
         <v>0.4</v>
@@ -3018,8 +3058,8 @@
       <c r="I66">
         <v>17546.759999999998</v>
       </c>
-      <c r="J66">
-        <v>17546.759999999998</v>
+      <c r="J66" s="2">
+        <v>0.75</v>
       </c>
       <c r="K66">
         <v>-0.4</v>
@@ -3056,8 +3096,8 @@
       <c r="I67">
         <v>44130.55</v>
       </c>
-      <c r="J67">
-        <v>44130.55</v>
+      <c r="J67" s="4">
+        <v>1.02</v>
       </c>
       <c r="K67">
         <v>0.6</v>
@@ -3091,8 +3131,8 @@
       <c r="H68">
         <v>92.5</v>
       </c>
-      <c r="J68">
-        <v>38952.93</v>
+      <c r="J68" s="2">
+        <v>1.0900000000000001</v>
       </c>
       <c r="K68">
         <v>-3.4</v>
@@ -3129,8 +3169,8 @@
       <c r="I69">
         <v>14949.62</v>
       </c>
-      <c r="J69">
-        <v>14949.62</v>
+      <c r="J69" s="4">
+        <v>0.86</v>
       </c>
       <c r="K69">
         <v>5.5</v>
@@ -3167,8 +3207,8 @@
       <c r="I70">
         <v>13519.69</v>
       </c>
-      <c r="J70">
-        <v>13519.69</v>
+      <c r="J70" s="2">
+        <v>0.81</v>
       </c>
       <c r="K70">
         <v>4.5</v>
@@ -3205,8 +3245,8 @@
       <c r="I71">
         <v>86661.14</v>
       </c>
-      <c r="J71">
-        <v>86661.14</v>
+      <c r="J71" s="4">
+        <v>1.29</v>
       </c>
       <c r="K71">
         <v>1.8</v>
@@ -3243,8 +3283,8 @@
       <c r="I72">
         <v>15211</v>
       </c>
-      <c r="J72">
-        <v>15211</v>
+      <c r="J72" s="2">
+        <v>0.64</v>
       </c>
       <c r="K72">
         <v>0.5</v>
@@ -3281,8 +3321,8 @@
       <c r="I73">
         <v>34225.9</v>
       </c>
-      <c r="J73">
-        <v>34225.9</v>
+      <c r="J73" s="4">
+        <v>1.1200000000000001</v>
       </c>
       <c r="K73">
         <v>0.1</v>
@@ -3319,8 +3359,8 @@
       <c r="I74">
         <v>73117.009999999995</v>
       </c>
-      <c r="J74">
-        <v>73117.009999999995</v>
+      <c r="J74" s="2">
+        <v>1.21</v>
       </c>
       <c r="K74">
         <v>-1</v>
@@ -3357,8 +3397,8 @@
       <c r="I75">
         <v>62307.65</v>
       </c>
-      <c r="J75">
-        <v>62307.65</v>
+      <c r="J75" s="4">
+        <v>0.96</v>
       </c>
       <c r="K75">
         <v>1.6</v>
@@ -3395,8 +3435,8 @@
       <c r="I76">
         <v>17083.54</v>
       </c>
-      <c r="J76">
-        <v>17083.54</v>
+      <c r="J76" s="2">
+        <v>0.71</v>
       </c>
       <c r="K76">
         <v>-0.5</v>
@@ -3433,8 +3473,8 @@
       <c r="I77">
         <v>24632.240000000002</v>
       </c>
-      <c r="J77">
-        <v>24632.240000000002</v>
+      <c r="J77" s="4">
+        <v>0.86</v>
       </c>
       <c r="K77">
         <v>0.6</v>
@@ -3471,8 +3511,8 @@
       <c r="I78">
         <v>10709.01</v>
       </c>
-      <c r="J78">
-        <v>10709.01</v>
+      <c r="J78" s="2">
+        <v>0.59</v>
       </c>
       <c r="K78">
         <v>-2.7</v>
@@ -3509,8 +3549,8 @@
       <c r="I79">
         <v>26367.63</v>
       </c>
-      <c r="J79">
-        <v>26367.63</v>
+      <c r="J79" s="4">
+        <v>0.88</v>
       </c>
       <c r="K79">
         <v>0.1</v>
@@ -3547,8 +3587,8 @@
       <c r="I80">
         <v>17931.82</v>
       </c>
-      <c r="J80">
-        <v>17931.82</v>
+      <c r="J80" s="2">
+        <v>0.62</v>
       </c>
       <c r="K80">
         <v>0.3</v>
@@ -3585,8 +3625,8 @@
       <c r="I81">
         <v>62322.22</v>
       </c>
-      <c r="J81">
-        <v>62322.22</v>
+      <c r="J81" s="4">
+        <v>1.1299999999999999</v>
       </c>
       <c r="K81">
         <v>0.8</v>
@@ -3623,8 +3663,8 @@
       <c r="I82">
         <v>69666.33</v>
       </c>
-      <c r="J82">
-        <v>69666.33</v>
+      <c r="J82" s="2">
+        <v>1.19</v>
       </c>
       <c r="K82">
         <v>-0.3</v>
@@ -3661,8 +3701,8 @@
       <c r="I83">
         <v>60218.27</v>
       </c>
-      <c r="J83">
-        <v>60218.27</v>
+      <c r="J83" s="2">
+        <v>1.05</v>
       </c>
       <c r="K83">
         <v>0.4</v>
@@ -3699,8 +3739,8 @@
       <c r="I84">
         <v>9419.01</v>
       </c>
-      <c r="J84">
-        <v>9419.01</v>
+      <c r="J84" s="4">
+        <v>0.63</v>
       </c>
       <c r="K84">
         <v>3.2</v>
@@ -3737,8 +3777,8 @@
       <c r="I85">
         <v>20926.060000000001</v>
       </c>
-      <c r="J85">
-        <v>20926.060000000001</v>
+      <c r="J85" s="2">
+        <v>0.81</v>
       </c>
       <c r="K85">
         <v>3.3</v>
@@ -3775,8 +3815,8 @@
       <c r="I86">
         <v>73498.41</v>
       </c>
-      <c r="J86">
-        <v>73498.41</v>
+      <c r="J86" s="4">
+        <v>1.2</v>
       </c>
       <c r="K86">
         <v>-0.4</v>
@@ -3813,8 +3853,8 @@
       <c r="I87">
         <v>63336.22</v>
       </c>
-      <c r="J87">
-        <v>63336.22</v>
+      <c r="J87" s="2">
+        <v>1.1100000000000001</v>
       </c>
       <c r="K87">
         <v>1.2</v>
@@ -3851,8 +3891,8 @@
       <c r="I88">
         <v>24479.02</v>
       </c>
-      <c r="J88">
-        <v>24479.02</v>
+      <c r="J88" s="5">
+        <v>1</v>
       </c>
       <c r="K88">
         <v>4.0999999999999996</v>
@@ -3889,8 +3929,8 @@
       <c r="I89">
         <v>70053.899999999994</v>
       </c>
-      <c r="J89">
-        <v>70053.899999999994</v>
+      <c r="J89" s="2">
+        <v>1.33</v>
       </c>
       <c r="K89">
         <v>4.9000000000000004</v>
@@ -3927,8 +3967,8 @@
       <c r="I90">
         <v>32722.74</v>
       </c>
-      <c r="J90">
-        <v>32722.74</v>
+      <c r="J90" s="4">
+        <v>0.79</v>
       </c>
       <c r="K90">
         <v>-1.2</v>
@@ -3965,8 +4005,8 @@
       <c r="I91">
         <v>42624.04</v>
       </c>
-      <c r="J91">
-        <v>42624.04</v>
+      <c r="J91" s="2">
+        <v>0.97</v>
       </c>
       <c r="K91">
         <v>-0.7</v>
@@ -4003,8 +4043,8 @@
       <c r="I92">
         <v>56827</v>
       </c>
-      <c r="J92">
-        <v>56827</v>
+      <c r="J92" s="4">
+        <v>0.99</v>
       </c>
       <c r="K92">
         <v>0.8</v>
@@ -4041,8 +4081,8 @@
       <c r="I93">
         <v>17873.45</v>
       </c>
-      <c r="J93">
-        <v>17873.45</v>
+      <c r="J93" s="2">
+        <v>0.79</v>
       </c>
       <c r="K93">
         <v>-2.2000000000000002</v>
@@ -4079,8 +4119,8 @@
       <c r="I94">
         <v>44208.62</v>
       </c>
-      <c r="J94">
-        <v>44208.62</v>
+      <c r="J94" s="4">
+        <v>1.03</v>
       </c>
       <c r="K94">
         <v>0.1</v>
@@ -4114,8 +4154,8 @@
       <c r="H95">
         <v>92</v>
       </c>
-      <c r="J95">
-        <v>38952.93</v>
+      <c r="J95" s="2">
+        <v>1.1200000000000001</v>
       </c>
       <c r="K95">
         <v>-3</v>
@@ -4152,8 +4192,8 @@
       <c r="I96">
         <v>15800.14</v>
       </c>
-      <c r="J96">
-        <v>15800.14</v>
+      <c r="J96" s="4">
+        <v>0.88</v>
       </c>
       <c r="K96">
         <v>4</v>
@@ -4190,8 +4230,8 @@
       <c r="I97">
         <v>14866.49</v>
       </c>
-      <c r="J97">
-        <v>14866.49</v>
+      <c r="J97" s="2">
+        <v>0.83</v>
       </c>
       <c r="K97">
         <v>5.5</v>
@@ -4228,8 +4268,8 @@
       <c r="I98">
         <v>87250.16</v>
       </c>
-      <c r="J98">
-        <v>87250.16</v>
+      <c r="J98" s="4">
+        <v>1.29</v>
       </c>
       <c r="K98">
         <v>-1.2</v>
@@ -4266,8 +4306,8 @@
       <c r="I99">
         <v>16265.59</v>
       </c>
-      <c r="J99">
-        <v>16265.59</v>
+      <c r="J99" s="2">
+        <v>0.66</v>
       </c>
       <c r="K99">
         <v>3.7</v>
@@ -4304,8 +4344,8 @@
       <c r="I100">
         <v>35402.400000000001</v>
       </c>
-      <c r="J100">
-        <v>35402.400000000001</v>
+      <c r="J100" s="4">
+        <v>1.1399999999999999</v>
       </c>
       <c r="K100">
         <v>4.5</v>
@@ -4342,8 +4382,8 @@
       <c r="I101">
         <v>74640.399999999994</v>
       </c>
-      <c r="J101">
-        <v>74640.399999999994</v>
+      <c r="J101" s="2">
+        <v>1.22</v>
       </c>
       <c r="K101">
         <v>1.2</v>
@@ -4380,8 +4420,8 @@
       <c r="I102">
         <v>66783.240000000005</v>
       </c>
-      <c r="J102">
-        <v>66783.240000000005</v>
+      <c r="J102" s="4">
+        <v>0.96</v>
       </c>
       <c r="K102">
         <v>1.5</v>
@@ -4418,8 +4458,8 @@
       <c r="I103">
         <v>17941.939999999999</v>
       </c>
-      <c r="J103">
-        <v>17941.939999999999</v>
+      <c r="J103" s="2">
+        <v>0.76</v>
       </c>
       <c r="K103">
         <v>2.6</v>
@@ -4456,8 +4496,8 @@
       <c r="I104">
         <v>24702.240000000002</v>
       </c>
-      <c r="J104">
-        <v>24702.240000000002</v>
+      <c r="J104" s="4">
+        <v>0.9</v>
       </c>
       <c r="K104">
         <v>0.9</v>
@@ -4494,8 +4534,8 @@
       <c r="I105">
         <v>11499.93</v>
       </c>
-      <c r="J105">
-        <v>11499.93</v>
+      <c r="J105" s="2">
+        <v>0.61</v>
       </c>
       <c r="K105">
         <v>11.8</v>
@@ -4532,8 +4572,8 @@
       <c r="I106">
         <v>26793.42</v>
       </c>
-      <c r="J106">
-        <v>26793.42</v>
+      <c r="J106" s="4">
+        <v>0.91</v>
       </c>
       <c r="K106">
         <v>2.5</v>
@@ -4570,8 +4610,8 @@
       <c r="I107">
         <v>18387</v>
       </c>
-      <c r="J107">
-        <v>18387</v>
+      <c r="J107" s="2">
+        <v>0.66</v>
       </c>
       <c r="K107">
         <v>2.7</v>
@@ -4608,8 +4648,8 @@
       <c r="I108">
         <v>63088.1</v>
       </c>
-      <c r="J108">
-        <v>63088.1</v>
+      <c r="J108" s="4">
+        <v>1.1399999999999999</v>
       </c>
       <c r="K108">
         <v>-1</v>
@@ -4646,8 +4686,8 @@
       <c r="I109">
         <v>70275.320000000007</v>
       </c>
-      <c r="J109">
-        <v>70275.320000000007</v>
+      <c r="J109" s="2">
+        <v>1.17</v>
       </c>
       <c r="K109">
         <v>1.9</v>
@@ -4684,8 +4724,8 @@
       <c r="I110">
         <v>61659.43</v>
       </c>
-      <c r="J110">
-        <v>61659.43</v>
+      <c r="J110" s="2">
+        <v>1.08</v>
       </c>
       <c r="K110">
         <v>1.8</v>
@@ -4722,8 +4762,8 @@
       <c r="I111">
         <v>10306.379999999999</v>
       </c>
-      <c r="J111">
-        <v>10306.379999999999</v>
+      <c r="J111" s="4">
+        <v>0.64</v>
       </c>
       <c r="K111">
         <v>9.5</v>
@@ -4760,8 +4800,8 @@
       <c r="I112">
         <v>22190.65</v>
       </c>
-      <c r="J112">
-        <v>22190.65</v>
+      <c r="J112" s="2">
+        <v>0.82</v>
       </c>
       <c r="K112">
         <v>3.8</v>
@@ -4798,8 +4838,8 @@
       <c r="I113">
         <v>74590.8</v>
       </c>
-      <c r="J113">
-        <v>74590.8</v>
+      <c r="J113" s="4">
+        <v>1.21</v>
       </c>
       <c r="K113">
         <v>0</v>
@@ -4836,8 +4876,8 @@
       <c r="I114">
         <v>64387.13</v>
       </c>
-      <c r="J114">
-        <v>64387.13</v>
+      <c r="J114" s="2">
+        <v>1.0900000000000001</v>
       </c>
       <c r="K114">
         <v>1.2</v>
@@ -4874,8 +4914,8 @@
       <c r="I115">
         <v>27116.49</v>
       </c>
-      <c r="J115">
-        <v>27116.49</v>
+      <c r="J115" s="5">
+        <v>1</v>
       </c>
       <c r="K115">
         <v>3.6</v>
@@ -4912,8 +4952,8 @@
       <c r="I116">
         <v>71313.16</v>
       </c>
-      <c r="J116">
-        <v>71313.16</v>
+      <c r="J116" s="2">
+        <v>1.36</v>
       </c>
       <c r="K116">
         <v>-3.7</v>
@@ -4950,8 +4990,8 @@
       <c r="I117">
         <v>32467.279999999999</v>
       </c>
-      <c r="J117">
-        <v>32467.279999999999</v>
+      <c r="J117" s="4">
+        <v>0.81</v>
       </c>
       <c r="K117">
         <v>-0.1</v>
@@ -4988,8 +5028,8 @@
       <c r="I118">
         <v>42866.3</v>
       </c>
-      <c r="J118">
-        <v>42866.3</v>
+      <c r="J118" s="2">
+        <v>0.98</v>
       </c>
       <c r="K118">
         <v>0.3</v>
@@ -5026,8 +5066,8 @@
       <c r="I119">
         <v>57130.29</v>
       </c>
-      <c r="J119">
-        <v>57130.29</v>
+      <c r="J119" s="4">
+        <v>0.99</v>
       </c>
       <c r="K119">
         <v>0.9</v>
@@ -5064,8 +5104,8 @@
       <c r="I120">
         <v>19494.23</v>
       </c>
-      <c r="J120">
-        <v>19494.23</v>
+      <c r="J120" s="2">
+        <v>0.82</v>
       </c>
       <c r="K120">
         <v>-0.2</v>
@@ -5102,8 +5142,8 @@
       <c r="I121">
         <v>44311.57</v>
       </c>
-      <c r="J121">
-        <v>44311.57</v>
+      <c r="J121" s="4">
+        <v>1.0900000000000001</v>
       </c>
       <c r="K121">
         <v>-0.1</v>
@@ -5140,8 +5180,8 @@
       <c r="I122">
         <v>39822.44</v>
       </c>
-      <c r="J122">
-        <v>39822.44</v>
+      <c r="J122" s="2">
+        <v>1.1399999999999999</v>
       </c>
       <c r="K122">
         <v>1.2</v>
@@ -5178,8 +5218,8 @@
       <c r="I123">
         <v>16920.849999999999</v>
       </c>
-      <c r="J123">
-        <v>16920.849999999999</v>
+      <c r="J123" s="4">
+        <v>0.9</v>
       </c>
       <c r="K123">
         <v>3.9</v>
@@ -5216,8 +5256,8 @@
       <c r="I124">
         <v>16515.37</v>
       </c>
-      <c r="J124">
-        <v>16515.37</v>
+      <c r="J124" s="2">
+        <v>0.88</v>
       </c>
       <c r="K124">
         <v>4</v>
@@ -5254,8 +5294,8 @@
       <c r="I125">
         <v>92151.41</v>
       </c>
-      <c r="J125">
-        <v>92151.41</v>
+      <c r="J125" s="4">
+        <v>1.32</v>
       </c>
       <c r="K125">
         <v>5.2</v>
@@ -5292,8 +5332,8 @@
       <c r="I126">
         <v>18244.150000000001</v>
       </c>
-      <c r="J126">
-        <v>18244.150000000001</v>
+      <c r="J126" s="2">
+        <v>0.68</v>
       </c>
       <c r="K126">
         <v>4.3</v>
@@ -5330,8 +5370,8 @@
       <c r="I127">
         <v>36160.300000000003</v>
       </c>
-      <c r="J127">
-        <v>36160.300000000003</v>
+      <c r="J127" s="4">
+        <v>1.18</v>
       </c>
       <c r="K127">
         <v>-3.5</v>
@@ -5368,8 +5408,8 @@
       <c r="I128">
         <v>75568.759999999995</v>
       </c>
-      <c r="J128">
-        <v>75568.759999999995</v>
+      <c r="J128" s="2">
+        <v>1.24</v>
       </c>
       <c r="K128">
         <v>0.6</v>
@@ -5406,8 +5446,8 @@
       <c r="I129">
         <v>67768.69</v>
       </c>
-      <c r="J129">
-        <v>67768.69</v>
+      <c r="J129" s="4">
+        <v>0.95</v>
       </c>
       <c r="K129">
         <v>1.1000000000000001</v>
@@ -5444,8 +5484,8 @@
       <c r="I130">
         <v>19883.03</v>
       </c>
-      <c r="J130">
-        <v>19883.03</v>
+      <c r="J130" s="2">
+        <v>0.77</v>
       </c>
       <c r="K130">
         <v>1.6</v>
@@ -5482,8 +5522,8 @@
       <c r="I131">
         <v>25076.6</v>
       </c>
-      <c r="J131">
-        <v>25076.6</v>
+      <c r="J131" s="4">
+        <v>0.95</v>
       </c>
       <c r="K131">
         <v>1.9</v>
@@ -5520,8 +5560,8 @@
       <c r="I132">
         <v>12541.18</v>
       </c>
-      <c r="J132">
-        <v>12541.18</v>
+      <c r="J132" s="2">
+        <v>0.62</v>
       </c>
       <c r="K132">
         <v>8.5</v>
@@ -5558,8 +5598,8 @@
       <c r="I133">
         <v>27406.16</v>
       </c>
-      <c r="J133">
-        <v>27406.16</v>
+      <c r="J133" s="4">
+        <v>0.91</v>
       </c>
       <c r="K133">
         <v>0.7</v>
@@ -5596,8 +5636,8 @@
       <c r="I134">
         <v>19000.39</v>
       </c>
-      <c r="J134">
-        <v>19000.39</v>
+      <c r="J134" s="2">
+        <v>0.67</v>
       </c>
       <c r="K134">
         <v>4.7</v>
@@ -5634,8 +5674,8 @@
       <c r="I135">
         <v>64060.03</v>
       </c>
-      <c r="J135">
-        <v>64060.03</v>
+      <c r="J135" s="4">
+        <v>1.1100000000000001</v>
       </c>
       <c r="K135">
         <v>-3.2</v>
@@ -5672,8 +5712,8 @@
       <c r="I136">
         <v>70648.36</v>
       </c>
-      <c r="J136">
-        <v>70648.36</v>
+      <c r="J136" s="2">
+        <v>1.1499999999999999</v>
       </c>
       <c r="K136">
         <v>2.8</v>
@@ -5710,8 +5750,8 @@
       <c r="I137">
         <v>63774.71</v>
       </c>
-      <c r="J137">
-        <v>63774.71</v>
+      <c r="J137" s="2">
+        <v>1.05</v>
       </c>
       <c r="K137">
         <v>1.3</v>
@@ -5748,8 +5788,8 @@
       <c r="I138">
         <v>10935.1</v>
       </c>
-      <c r="J138">
-        <v>10935.1</v>
+      <c r="J138" s="4">
+        <v>0.66</v>
       </c>
       <c r="K138">
         <v>6.9</v>
@@ -5786,8 +5826,8 @@
       <c r="I139">
         <v>25189.31</v>
       </c>
-      <c r="J139">
-        <v>25189.31</v>
+      <c r="J139" s="2">
+        <v>0.84</v>
       </c>
       <c r="K139">
         <v>6.6</v>
@@ -5824,8 +5864,8 @@
       <c r="I140">
         <v>76082.789999999994</v>
       </c>
-      <c r="J140">
-        <v>76082.789999999994</v>
+      <c r="J140" s="4">
+        <v>1.2</v>
       </c>
       <c r="K140">
         <v>1.3</v>
@@ -5862,8 +5902,8 @@
       <c r="I141">
         <v>66383.77</v>
       </c>
-      <c r="J141">
-        <v>66383.77</v>
+      <c r="J141" s="2">
+        <v>1.0900000000000001</v>
       </c>
       <c r="K141">
         <v>3.2</v>
@@ -5900,8 +5940,8 @@
       <c r="I142">
         <v>28564.99</v>
       </c>
-      <c r="J142">
-        <v>28564.99</v>
+      <c r="J142" s="4">
+        <v>1.02</v>
       </c>
       <c r="K142">
         <v>7</v>
@@ -5938,8 +5978,8 @@
       <c r="I143">
         <v>73613.039999999994</v>
       </c>
-      <c r="J143">
-        <v>73613.039999999994</v>
+      <c r="J143" s="2">
+        <v>1.34</v>
       </c>
       <c r="K143">
         <v>-1.8</v>
@@ -5976,8 +6016,8 @@
       <c r="I144">
         <v>32437.22</v>
       </c>
-      <c r="J144">
-        <v>32437.22</v>
+      <c r="J144" s="4">
+        <v>0.85</v>
       </c>
       <c r="K144">
         <v>-1.4</v>
@@ -6014,8 +6054,8 @@
       <c r="I145">
         <v>43365.84</v>
       </c>
-      <c r="J145">
-        <v>43365.84</v>
+      <c r="J145" s="2">
+        <v>1.01</v>
       </c>
       <c r="K145">
         <v>1.6</v>
@@ -6052,8 +6092,8 @@
       <c r="I146">
         <v>58446.84</v>
       </c>
-      <c r="J146">
-        <v>58446.84</v>
+      <c r="J146" s="4">
+        <v>0.99</v>
       </c>
       <c r="K146">
         <v>0.8</v>
@@ -6090,8 +6130,8 @@
       <c r="I147">
         <v>20253.64</v>
       </c>
-      <c r="J147">
-        <v>20253.64</v>
+      <c r="J147" s="2">
+        <v>0.86</v>
       </c>
       <c r="K147">
         <v>3.7</v>
@@ -6128,8 +6168,8 @@
       <c r="I148">
         <v>44622.87</v>
       </c>
-      <c r="J148">
-        <v>44622.87</v>
+      <c r="J148" s="4">
+        <v>1.05</v>
       </c>
       <c r="K148">
         <v>1.5</v>
@@ -6166,8 +6206,8 @@
       <c r="I149">
         <v>40813.769999999997</v>
       </c>
-      <c r="J149">
-        <v>40813.769999999997</v>
+      <c r="J149" s="2">
+        <v>1.1499999999999999</v>
       </c>
       <c r="K149">
         <v>1.2</v>
@@ -6204,8 +6244,8 @@
       <c r="I150">
         <v>18419.32</v>
       </c>
-      <c r="J150">
-        <v>18419.32</v>
+      <c r="J150" s="4">
+        <v>0.9</v>
       </c>
       <c r="K150">
         <v>4.7</v>
@@ -6242,8 +6282,8 @@
       <c r="I151">
         <v>18101.310000000001</v>
       </c>
-      <c r="J151">
-        <v>18101.310000000001</v>
+      <c r="J151" s="2">
+        <v>0.91</v>
       </c>
       <c r="K151">
         <v>4.3</v>
@@ -6280,8 +6320,8 @@
       <c r="I152">
         <v>93618.46</v>
       </c>
-      <c r="J152">
-        <v>93618.46</v>
+      <c r="J152" s="4">
+        <v>1.31</v>
       </c>
       <c r="K152">
         <v>4.4000000000000004</v>
@@ -6318,8 +6358,8 @@
       <c r="I153">
         <v>19491.96</v>
       </c>
-      <c r="J153">
-        <v>19491.96</v>
+      <c r="J153" s="2">
+        <v>0.7</v>
       </c>
       <c r="K153">
         <v>2.8</v>
@@ -6356,8 +6396,8 @@
       <c r="I154">
         <v>37330.300000000003</v>
       </c>
-      <c r="J154">
-        <v>37330.300000000003</v>
+      <c r="J154" s="4">
+        <v>1.18</v>
       </c>
       <c r="K154">
         <v>7.3</v>
@@ -6394,8 +6434,8 @@
       <c r="I155">
         <v>76436.36</v>
       </c>
-      <c r="J155">
-        <v>76436.36</v>
+      <c r="J155" s="2">
+        <v>1.23</v>
       </c>
       <c r="K155">
         <v>2.7</v>
@@ -6432,8 +6472,8 @@
       <c r="I156">
         <v>68953.87</v>
       </c>
-      <c r="J156">
-        <v>68953.87</v>
+      <c r="J156" s="4">
+        <v>0.95</v>
       </c>
       <c r="K156">
         <v>2.4</v>
@@ -6470,8 +6510,8 @@
       <c r="I157">
         <v>21307.84</v>
       </c>
-      <c r="J157">
-        <v>21307.84</v>
+      <c r="J157" s="2">
+        <v>0.79</v>
       </c>
       <c r="K157">
         <v>1.7</v>
@@ -6508,8 +6548,8 @@
       <c r="I158">
         <v>26003.5</v>
       </c>
-      <c r="J158">
-        <v>26003.5</v>
+      <c r="J158" s="4">
+        <v>0.99</v>
       </c>
       <c r="K158">
         <v>3.7</v>
@@ -6546,8 +6586,8 @@
       <c r="I159">
         <v>13772.36</v>
       </c>
-      <c r="J159">
-        <v>13772.36</v>
+      <c r="J159" s="2">
+        <v>0.63</v>
       </c>
       <c r="K159">
         <v>6.3</v>
@@ -6584,8 +6624,8 @@
       <c r="I160">
         <v>27872.25</v>
       </c>
-      <c r="J160">
-        <v>27872.25</v>
+      <c r="J160" s="4">
+        <v>0.91</v>
       </c>
       <c r="K160">
         <v>2.7</v>
@@ -6622,8 +6662,8 @@
       <c r="I161">
         <v>20014.98</v>
       </c>
-      <c r="J161">
-        <v>20014.98</v>
+      <c r="J161" s="2">
+        <v>0.68</v>
       </c>
       <c r="K161">
         <v>3.8</v>
@@ -6660,8 +6700,8 @@
       <c r="I162">
         <v>65197.07</v>
       </c>
-      <c r="J162">
-        <v>65197.07</v>
+      <c r="J162" s="4">
+        <v>1.1299999999999999</v>
       </c>
       <c r="K162">
         <v>2.7</v>
@@ -6698,8 +6738,8 @@
       <c r="I163">
         <v>68398.66</v>
       </c>
-      <c r="J163">
-        <v>68398.66</v>
+      <c r="J163" s="2">
+        <v>1.1299999999999999</v>
       </c>
       <c r="K163">
         <v>3.6</v>
@@ -6736,8 +6776,8 @@
       <c r="I164">
         <v>65824.639999999999</v>
       </c>
-      <c r="J164">
-        <v>65824.639999999999</v>
+      <c r="J164" s="2">
+        <v>1.0900000000000001</v>
       </c>
       <c r="K164">
         <v>1.3</v>
@@ -6774,8 +6814,8 @@
       <c r="I165">
         <v>12226.94</v>
       </c>
-      <c r="J165">
-        <v>12226.94</v>
+      <c r="J165" s="4">
+        <v>0.69</v>
       </c>
       <c r="K165">
         <v>1.6</v>
@@ -6812,8 +6852,8 @@
       <c r="I166">
         <v>25853.61</v>
       </c>
-      <c r="J166">
-        <v>25853.61</v>
+      <c r="J166" s="2">
+        <v>0.84</v>
       </c>
       <c r="K166">
         <v>3.4</v>
@@ -6850,8 +6890,8 @@
       <c r="I167">
         <v>77753.350000000006</v>
       </c>
-      <c r="J167">
-        <v>77753.350000000006</v>
+      <c r="J167" s="4">
+        <v>1.23</v>
       </c>
       <c r="K167">
         <v>1</v>
@@ -6888,8 +6928,8 @@
       <c r="I168">
         <v>68681.649999999994</v>
       </c>
-      <c r="J168">
-        <v>68681.649999999994</v>
+      <c r="J168" s="2">
+        <v>1.0900000000000001</v>
       </c>
       <c r="K168">
         <v>3</v>
@@ -6926,8 +6966,8 @@
       <c r="I169">
         <v>30148.81</v>
       </c>
-      <c r="J169">
-        <v>30148.81</v>
+      <c r="J169" s="4">
+        <v>1.04</v>
       </c>
       <c r="K169">
         <v>5.3</v>
@@ -6964,8 +7004,8 @@
       <c r="I170">
         <v>79864.41</v>
       </c>
-      <c r="J170">
-        <v>79864.41</v>
+      <c r="J170" s="2">
+        <v>1.28</v>
       </c>
       <c r="K170">
         <v>2</v>
@@ -7002,8 +7042,8 @@
       <c r="I171">
         <v>33014.69</v>
       </c>
-      <c r="J171">
-        <v>33014.69</v>
+      <c r="J171" s="4">
+        <v>0.85</v>
       </c>
       <c r="K171">
         <v>-1</v>
@@ -7040,8 +7080,8 @@
       <c r="I172">
         <v>43907.18</v>
       </c>
-      <c r="J172">
-        <v>43907.18</v>
+      <c r="J172" s="3">
+        <v>1</v>
       </c>
       <c r="K172">
         <v>4.4000000000000004</v>
@@ -7078,8 +7118,8 @@
       <c r="I173">
         <v>59451.97</v>
       </c>
-      <c r="J173">
-        <v>59451.97</v>
+      <c r="J173" s="4">
+        <v>0.97</v>
       </c>
       <c r="K173">
         <v>-0.9</v>
@@ -7116,8 +7156,8 @@
       <c r="I174">
         <v>20773.919999999998</v>
       </c>
-      <c r="J174">
-        <v>20773.919999999998</v>
+      <c r="J174" s="2">
+        <v>0.85</v>
       </c>
       <c r="K174">
         <v>-1.2</v>
@@ -7154,8 +7194,8 @@
       <c r="I175">
         <v>45014.86</v>
       </c>
-      <c r="J175">
-        <v>45014.86</v>
+      <c r="J175" s="4">
+        <v>1.08</v>
       </c>
       <c r="K175">
         <v>1.5</v>
@@ -7192,8 +7232,8 @@
       <c r="I176">
         <v>41336.99</v>
       </c>
-      <c r="J176">
-        <v>41336.99</v>
+      <c r="J176" s="2">
+        <v>1.1399999999999999</v>
       </c>
       <c r="K176">
         <v>4.4000000000000004</v>
@@ -7230,8 +7270,8 @@
       <c r="I177">
         <v>19921.78</v>
       </c>
-      <c r="J177">
-        <v>19921.78</v>
+      <c r="J177" s="4">
+        <v>0.92</v>
       </c>
       <c r="K177">
         <v>6.7</v>
@@ -7268,8 +7308,8 @@
       <c r="I178">
         <v>20793.689999999999</v>
       </c>
-      <c r="J178">
-        <v>20793.689999999999</v>
+      <c r="J178" s="2">
+        <v>0.93</v>
       </c>
       <c r="K178">
         <v>6.1</v>
@@ -7306,8 +7346,8 @@
       <c r="I179">
         <v>94772.17</v>
       </c>
-      <c r="J179">
-        <v>94772.17</v>
+      <c r="J179" s="4">
+        <v>1.32</v>
       </c>
       <c r="K179">
         <v>2.7</v>
@@ -7344,8 +7384,8 @@
       <c r="I180">
         <v>21237.86</v>
       </c>
-      <c r="J180">
-        <v>21237.86</v>
+      <c r="J180" s="2">
+        <v>0.7</v>
       </c>
       <c r="K180">
         <v>4.5999999999999996</v>
@@ -7382,8 +7422,8 @@
       <c r="I181">
         <v>39764.379999999997</v>
       </c>
-      <c r="J181">
-        <v>39764.379999999997</v>
+      <c r="J181" s="4">
+        <v>1.18</v>
       </c>
       <c r="K181">
         <v>5.4</v>
@@ -7420,8 +7460,8 @@
       <c r="I182">
         <v>79787.48</v>
       </c>
-      <c r="J182">
-        <v>79787.48</v>
+      <c r="J182" s="2">
+        <v>1.17</v>
       </c>
       <c r="K182">
         <v>3.1</v>
@@ -7458,8 +7498,8 @@
       <c r="I183">
         <v>72818.240000000005</v>
       </c>
-      <c r="J183">
-        <v>72818.240000000005</v>
+      <c r="J183" s="4">
+        <v>0.95</v>
       </c>
       <c r="K183">
         <v>2</v>
@@ -7496,8 +7536,8 @@
       <c r="I184">
         <v>23202.880000000001</v>
       </c>
-      <c r="J184">
-        <v>23202.880000000001</v>
+      <c r="J184" s="2">
+        <v>0.79</v>
       </c>
       <c r="K184">
         <v>3.6</v>
@@ -7534,8 +7574,8 @@
       <c r="I185">
         <v>26846.799999999999</v>
       </c>
-      <c r="J185">
-        <v>26846.799999999999</v>
+      <c r="J185" s="4">
+        <v>1.02</v>
       </c>
       <c r="K185">
         <v>3.2</v>
@@ -7572,8 +7612,8 @@
       <c r="I186">
         <v>14885.58</v>
       </c>
-      <c r="J186">
-        <v>14885.58</v>
+      <c r="J186" s="2">
+        <v>0.62</v>
       </c>
       <c r="K186">
         <v>7.2</v>
@@ -7610,8 +7650,8 @@
       <c r="I187">
         <v>28723.48</v>
       </c>
-      <c r="J187">
-        <v>28723.48</v>
+      <c r="J187" s="4">
+        <v>0.89</v>
       </c>
       <c r="K187">
         <v>4.0999999999999996</v>
@@ -7648,8 +7688,8 @@
       <c r="I188">
         <v>21066.28</v>
       </c>
-      <c r="J188">
-        <v>21066.28</v>
+      <c r="J188" s="2">
+        <v>0.68</v>
       </c>
       <c r="K188">
         <v>5.6</v>
@@ -7686,8 +7726,8 @@
       <c r="I189">
         <v>66666.91</v>
       </c>
-      <c r="J189">
-        <v>66666.91</v>
+      <c r="J189" s="4">
+        <v>1.1200000000000001</v>
       </c>
       <c r="K189">
         <v>1.8</v>
@@ -7724,8 +7764,8 @@
       <c r="I190">
         <v>67858.27</v>
       </c>
-      <c r="J190">
-        <v>67858.27</v>
+      <c r="J190" s="2">
+        <v>1.1200000000000001</v>
       </c>
       <c r="K190">
         <v>1</v>
@@ -7762,8 +7802,8 @@
       <c r="I191">
         <v>66552.41</v>
       </c>
-      <c r="J191">
-        <v>66552.41</v>
+      <c r="J191" s="2">
+        <v>1.04</v>
       </c>
       <c r="K191">
         <v>1.5</v>
@@ -7800,8 +7840,8 @@
       <c r="I192">
         <v>13266.45</v>
       </c>
-      <c r="J192">
-        <v>13266.45</v>
+      <c r="J192" s="4">
+        <v>0.66</v>
       </c>
       <c r="K192">
         <v>8.5</v>
@@ -7838,8 +7878,8 @@
       <c r="I193">
         <v>26634.41</v>
       </c>
-      <c r="J193">
-        <v>26634.41</v>
+      <c r="J193" s="2">
+        <v>0.81</v>
       </c>
       <c r="K193">
         <v>7.2</v>
@@ -7876,8 +7916,8 @@
       <c r="I194">
         <v>79278.41</v>
       </c>
-      <c r="J194">
-        <v>79278.41</v>
+      <c r="J194" s="4">
+        <v>1.2</v>
       </c>
       <c r="K194">
         <v>3.2</v>
@@ -7914,8 +7954,8 @@
       <c r="I195">
         <v>68534.23</v>
       </c>
-      <c r="J195">
-        <v>68534.23</v>
+      <c r="J195" s="2">
+        <v>1.06</v>
       </c>
       <c r="K195">
         <v>3.2</v>
@@ -7952,8 +7992,8 @@
       <c r="I196">
         <v>30698.84</v>
       </c>
-      <c r="J196">
-        <v>30698.84</v>
+      <c r="J196" s="4">
+        <v>0.98</v>
       </c>
       <c r="K196">
         <v>4.4000000000000004</v>
@@ -7990,8 +8030,8 @@
       <c r="I197">
         <v>81045.42</v>
       </c>
-      <c r="J197">
-        <v>81045.42</v>
+      <c r="J197" s="2">
+        <v>1.23</v>
       </c>
       <c r="K197">
         <v>-8.4</v>
@@ -8028,8 +8068,8 @@
       <c r="I198">
         <v>31074.14</v>
       </c>
-      <c r="J198">
-        <v>31074.14</v>
+      <c r="J198" s="4">
+        <v>0.77</v>
       </c>
       <c r="K198">
         <v>7.2</v>
@@ -8066,8 +8106,8 @@
       <c r="I199">
         <v>42209.15</v>
       </c>
-      <c r="J199">
-        <v>42209.15</v>
+      <c r="J199" s="2">
+        <v>0.91</v>
       </c>
       <c r="K199">
         <v>6.4</v>
@@ -8104,8 +8144,8 @@
       <c r="I200">
         <v>58096.82</v>
       </c>
-      <c r="J200">
-        <v>58096.82</v>
+      <c r="J200" s="4">
+        <v>0.92</v>
       </c>
       <c r="K200">
         <v>4.4000000000000004</v>
@@ -8142,8 +8182,8 @@
       <c r="I201">
         <v>21548.9</v>
       </c>
-      <c r="J201">
-        <v>21548.9</v>
+      <c r="J201" s="2">
+        <v>0.81</v>
       </c>
       <c r="K201">
         <v>8.9</v>
@@ -8180,8 +8220,8 @@
       <c r="I202">
         <v>47426.32</v>
       </c>
-      <c r="J202">
-        <v>47426.32</v>
+      <c r="J202" s="5">
+        <v>1</v>
       </c>
       <c r="K202">
         <v>1.9</v>
@@ -8218,8 +8258,8 @@
       <c r="I203">
         <v>40888.57</v>
       </c>
-      <c r="J203">
-        <v>40888.57</v>
+      <c r="J203" s="3">
+        <v>1</v>
       </c>
       <c r="K203">
         <v>3.5</v>
@@ -8256,8 +8296,8 @@
       <c r="I204">
         <v>21303.37</v>
       </c>
-      <c r="J204">
-        <v>21303.37</v>
+      <c r="J204" s="4">
+        <v>0.9</v>
       </c>
       <c r="K204">
         <v>5.0999999999999996</v>
@@ -8294,8 +8334,8 @@
       <c r="I205">
         <v>23256.57</v>
       </c>
-      <c r="J205">
-        <v>23256.57</v>
+      <c r="J205" s="2">
+        <v>0.92</v>
       </c>
       <c r="K205">
         <v>4.0999999999999996</v>
@@ -8332,8 +8372,8 @@
       <c r="I206">
         <v>98219.38</v>
       </c>
-      <c r="J206">
-        <v>98219.38</v>
+      <c r="J206" s="4">
+        <v>1.27</v>
       </c>
       <c r="K206">
         <v>3.2</v>
@@ -8370,8 +8410,8 @@
       <c r="I207">
         <v>21373.69</v>
       </c>
-      <c r="J207">
-        <v>21373.69</v>
+      <c r="J207" s="2">
+        <v>0.68</v>
       </c>
       <c r="K207">
         <v>6.1</v>
@@ -8408,8 +8448,8 @@
       <c r="I208">
         <v>40855.800000000003</v>
       </c>
-      <c r="J208">
-        <v>40855.800000000003</v>
+      <c r="J208" s="4">
+        <v>1.08</v>
       </c>
       <c r="K208">
         <v>7.4</v>
@@ -8446,8 +8486,8 @@
       <c r="I209">
         <v>83321.740000000005</v>
       </c>
-      <c r="J209">
-        <v>83321.740000000005</v>
+      <c r="J209" s="2">
+        <v>1.08</v>
       </c>
       <c r="K209">
         <v>6.9</v>
@@ -8484,8 +8524,8 @@
       <c r="I210">
         <v>74952.73</v>
       </c>
-      <c r="J210">
-        <v>74952.73</v>
+      <c r="J210" s="4">
+        <v>0.94</v>
       </c>
       <c r="K210">
         <v>7.2</v>
@@ -8522,8 +8562,8 @@
       <c r="I211">
         <v>26089.21</v>
       </c>
-      <c r="J211">
-        <v>26089.21</v>
+      <c r="J211" s="2">
+        <v>0.81</v>
       </c>
       <c r="K211">
         <v>6.9</v>
@@ -8560,8 +8600,8 @@
       <c r="I212">
         <v>27069.57</v>
       </c>
-      <c r="J212">
-        <v>27069.57</v>
+      <c r="J212" s="4">
+        <v>0.94</v>
       </c>
       <c r="K212">
         <v>7.9</v>
@@ -8598,8 +8638,8 @@
       <c r="I213">
         <v>16003.32</v>
       </c>
-      <c r="J213">
-        <v>16003.32</v>
+      <c r="J213" s="2">
+        <v>0.62</v>
       </c>
       <c r="K213">
         <v>6.2</v>
@@ -8636,8 +8676,8 @@
       <c r="I214">
         <v>29889.63</v>
       </c>
-      <c r="J214">
-        <v>29889.63</v>
+      <c r="J214" s="4">
+        <v>0.85</v>
       </c>
       <c r="K214">
         <v>7</v>
@@ -8674,8 +8714,8 @@
       <c r="I215">
         <v>21645.759999999998</v>
       </c>
-      <c r="J215">
-        <v>21645.759999999998</v>
+      <c r="J215" s="2">
+        <v>0.67</v>
       </c>
       <c r="K215">
         <v>4</v>
@@ -8712,8 +8752,8 @@
       <c r="I216">
         <v>68780.600000000006</v>
       </c>
-      <c r="J216">
-        <v>68780.600000000006</v>
+      <c r="J216" s="4">
+        <v>1.07</v>
       </c>
       <c r="K216">
         <v>0.6</v>
@@ -8750,8 +8790,8 @@
       <c r="I217">
         <v>69766.33</v>
       </c>
-      <c r="J217">
-        <v>69766.33</v>
+      <c r="J217" s="3">
+        <v>1</v>
       </c>
       <c r="K217">
         <v>3.1</v>
@@ -8788,8 +8828,8 @@
       <c r="I218">
         <v>67709.66</v>
       </c>
-      <c r="J218">
-        <v>67709.66</v>
+      <c r="J218" s="2">
+        <v>1.03</v>
       </c>
       <c r="K218">
         <v>2.2999999999999998</v>
@@ -8826,8 +8866,8 @@
       <c r="I219">
         <v>15833.69</v>
       </c>
-      <c r="J219">
-        <v>15833.69</v>
+      <c r="J219" s="4">
+        <v>0.69</v>
       </c>
       <c r="K219">
         <v>3.4</v>
@@ -8864,8 +8904,8 @@
       <c r="I220">
         <v>29995.8</v>
       </c>
-      <c r="J220">
-        <v>29995.8</v>
+      <c r="J220" s="2">
+        <v>0.88</v>
       </c>
       <c r="K220">
         <v>3.6</v>
@@ -8902,8 +8942,8 @@
       <c r="I221">
         <v>82185.88</v>
       </c>
-      <c r="J221">
-        <v>82185.88</v>
+      <c r="J221" s="4">
+        <v>1.18</v>
       </c>
       <c r="K221">
         <v>-1.3</v>
@@ -8940,8 +8980,8 @@
       <c r="I222">
         <v>71564.399999999994</v>
       </c>
-      <c r="J222">
-        <v>71564.399999999994</v>
+      <c r="J222" s="2">
+        <v>1.03</v>
       </c>
       <c r="K222">
         <v>-0.3</v>
@@ -8978,8 +9018,8 @@
       <c r="I223">
         <v>32410.48</v>
       </c>
-      <c r="J223">
-        <v>32410.48</v>
+      <c r="J223" s="4">
+        <v>0.99</v>
       </c>
       <c r="K223">
         <v>2.2000000000000002</v>
@@ -9016,8 +9056,8 @@
       <c r="I224">
         <v>83220.63</v>
       </c>
-      <c r="J224">
-        <v>83220.63</v>
+      <c r="J224" s="2">
+        <v>1.18</v>
       </c>
       <c r="K224">
         <v>-5</v>
@@ -9054,8 +9094,8 @@
       <c r="I225">
         <v>33680.120000000003</v>
       </c>
-      <c r="J225">
-        <v>33680.120000000003</v>
+      <c r="J225" s="4">
+        <v>0.82</v>
       </c>
       <c r="K225">
         <v>-1.7</v>
@@ -9092,8 +9132,8 @@
       <c r="I226">
         <v>44280.53</v>
       </c>
-      <c r="J226">
-        <v>44280.53</v>
+      <c r="J226" s="3">
+        <v>1</v>
       </c>
       <c r="K226">
         <v>1.7</v>
@@ -9130,8 +9170,8 @@
       <c r="I227">
         <v>60476.18</v>
       </c>
-      <c r="J227">
-        <v>60476.18</v>
+      <c r="J227" s="4">
+        <v>0.94</v>
       </c>
       <c r="K227">
         <v>0.4</v>
@@ -9168,8 +9208,8 @@
       <c r="I228">
         <v>22362.76</v>
       </c>
-      <c r="J228">
-        <v>22362.76</v>
+      <c r="J228" s="2">
+        <v>0.87</v>
       </c>
       <c r="K228">
         <v>-5</v>
@@ -9206,8 +9246,8 @@
       <c r="I229">
         <v>49376.800000000003</v>
       </c>
-      <c r="J229">
-        <v>49376.800000000003</v>
+      <c r="J229" s="4">
+        <v>1.04</v>
       </c>
       <c r="K229">
         <v>0.1</v>
@@ -9244,8 +9284,8 @@
       <c r="I230">
         <v>41693.019999999997</v>
       </c>
-      <c r="J230">
-        <v>41693.019999999997</v>
+      <c r="J230" s="2">
+        <v>1.05</v>
       </c>
       <c r="K230">
         <v>-3.9</v>
@@ -9282,8 +9322,8 @@
       <c r="I231">
         <v>24188.67</v>
       </c>
-      <c r="J231">
-        <v>24188.67</v>
+      <c r="J231" s="4">
+        <v>0.88</v>
       </c>
       <c r="K231">
         <v>-0.8</v>
@@ -9320,8 +9360,8 @@
       <c r="I232">
         <v>25276.42</v>
       </c>
-      <c r="J232">
-        <v>25276.42</v>
+      <c r="J232" s="2">
+        <v>0.95</v>
       </c>
       <c r="K232">
         <v>6.4</v>
@@ -9358,8 +9398,8 @@
       <c r="I233">
         <v>99361.25</v>
       </c>
-      <c r="J233">
-        <v>99361.25</v>
+      <c r="J233" s="4">
+        <v>1.31</v>
       </c>
       <c r="K233">
         <v>1.4</v>
@@ -9396,8 +9436,8 @@
       <c r="I234">
         <v>22379.05</v>
       </c>
-      <c r="J234">
-        <v>22379.05</v>
+      <c r="J234" s="2">
+        <v>0.71</v>
       </c>
       <c r="K234">
         <v>3.3</v>
@@ -9434,8 +9474,8 @@
       <c r="I235">
         <v>38235</v>
       </c>
-      <c r="J235">
-        <v>38235</v>
+      <c r="J235" s="4">
+        <v>1.1100000000000001</v>
       </c>
       <c r="K235">
         <v>-4.5999999999999996</v>
@@ -9472,8 +9512,8 @@
       <c r="I236">
         <v>86316.92</v>
       </c>
-      <c r="J236">
-        <v>86316.92</v>
+      <c r="J236" s="2">
+        <v>1.1000000000000001</v>
       </c>
       <c r="K236">
         <v>-1.4</v>
@@ -9510,8 +9550,8 @@
       <c r="I237">
         <v>75592.41</v>
       </c>
-      <c r="J237">
-        <v>75592.41</v>
+      <c r="J237" s="4">
+        <v>0.94</v>
       </c>
       <c r="K237">
         <v>-0.5</v>
@@ -9548,8 +9588,8 @@
       <c r="I238">
         <v>25516.32</v>
       </c>
-      <c r="J238">
-        <v>25516.32</v>
+      <c r="J238" s="2">
+        <v>0.85</v>
       </c>
       <c r="K238">
         <v>1.5</v>
@@ -9586,8 +9626,8 @@
       <c r="I239">
         <v>28205.08</v>
       </c>
-      <c r="J239">
-        <v>28205.08</v>
+      <c r="J239" s="4">
+        <v>0.97</v>
       </c>
       <c r="K239">
         <v>1</v>
@@ -9624,8 +9664,8 @@
       <c r="I240">
         <v>17183.22</v>
       </c>
-      <c r="J240">
-        <v>17183.22</v>
+      <c r="J240" s="2">
+        <v>0.64</v>
       </c>
       <c r="K240">
         <v>1.8</v>
@@ -9662,8 +9702,8 @@
       <c r="I241">
         <v>31367.01</v>
       </c>
-      <c r="J241">
-        <v>31367.01</v>
+      <c r="J241" s="4">
+        <v>0.84</v>
       </c>
       <c r="K241">
         <v>0.5</v>
@@ -9700,8 +9740,8 @@
       <c r="I242">
         <v>23329.279999999999</v>
       </c>
-      <c r="J242">
-        <v>23329.279999999999</v>
+      <c r="J242" s="2">
+        <v>0.69</v>
       </c>
       <c r="K242">
         <v>0.3</v>
@@ -9738,8 +9778,8 @@
       <c r="I243">
         <v>70208.929999999993</v>
       </c>
-      <c r="J243">
-        <v>70208.929999999993</v>
+      <c r="J243" s="4">
+        <v>1.08</v>
       </c>
       <c r="K243">
         <v>3.8</v>
@@ -9776,8 +9816,8 @@
       <c r="I244">
         <v>74105.55</v>
       </c>
-      <c r="J244">
-        <v>74105.55</v>
+      <c r="J244" s="2">
+        <v>1.02</v>
       </c>
       <c r="K244">
         <v>-0.2</v>
@@ -9814,8 +9854,8 @@
       <c r="I245">
         <v>71793.7</v>
       </c>
-      <c r="J245">
-        <v>71793.7</v>
+      <c r="J245" s="2">
+        <v>1.05</v>
       </c>
       <c r="K245">
         <v>5.2</v>
@@ -9852,8 +9892,8 @@
       <c r="I246">
         <v>18058.71</v>
       </c>
-      <c r="J246">
-        <v>18058.71</v>
+      <c r="J246" s="4">
+        <v>0.7</v>
       </c>
       <c r="K246">
         <v>10.6</v>
@@ -9890,8 +9930,8 @@
       <c r="I247">
         <v>33593.019999999997</v>
       </c>
-      <c r="J247">
-        <v>33593.019999999997</v>
+      <c r="J247" s="2">
+        <v>0.91</v>
       </c>
       <c r="K247">
         <v>5.4</v>
@@ -9928,8 +9968,8 @@
       <c r="I248">
         <v>85005.759999999995</v>
       </c>
-      <c r="J248">
-        <v>85005.759999999995</v>
+      <c r="J248" s="4">
+        <v>1.22</v>
       </c>
       <c r="K248">
         <v>5</v>
@@ -9966,8 +10006,8 @@
       <c r="I249">
         <v>77469.09</v>
       </c>
-      <c r="J249">
-        <v>77469.09</v>
+      <c r="J249" s="2">
+        <v>1.05</v>
       </c>
       <c r="K249">
         <v>4.4000000000000004</v>
@@ -10004,8 +10044,8 @@
       <c r="I250">
         <v>34753.79</v>
       </c>
-      <c r="J250">
-        <v>34753.79</v>
+      <c r="J250" s="5">
+        <v>1</v>
       </c>
       <c r="K250">
         <v>12.7</v>
@@ -10042,8 +10082,8 @@
       <c r="I251">
         <v>85765.82</v>
       </c>
-      <c r="J251">
-        <v>85765.82</v>
+      <c r="J251" s="2">
+        <v>1.21</v>
       </c>
       <c r="K251">
         <v>1.2</v>
@@ -10080,8 +10120,8 @@
       <c r="I252">
         <v>36666.660000000003</v>
       </c>
-      <c r="J252">
-        <v>36666.660000000003</v>
+      <c r="J252" s="4">
+        <v>0.89</v>
       </c>
       <c r="K252">
         <v>-1.8</v>
@@ -10118,8 +10158,8 @@
       <c r="I253">
         <v>46073.19</v>
       </c>
-      <c r="J253">
-        <v>46073.19</v>
+      <c r="J253" s="2">
+        <v>1.07</v>
       </c>
       <c r="K253">
         <v>1.9</v>
@@ -10156,8 +10196,8 @@
       <c r="I254">
         <v>63799.45</v>
       </c>
-      <c r="J254">
-        <v>63799.45</v>
+      <c r="J254" s="4">
+        <v>0.97</v>
       </c>
       <c r="K254">
         <v>4.7</v>
@@ -10194,8 +10234,8 @@
       <c r="I255">
         <v>24046.49</v>
       </c>
-      <c r="J255">
-        <v>24046.49</v>
+      <c r="J255" s="2">
+        <v>0.91</v>
       </c>
       <c r="K255">
         <v>7.3</v>
@@ -10232,8 +10272,8 @@
       <c r="I256">
         <v>51762.53</v>
       </c>
-      <c r="J256">
-        <v>51762.53</v>
+      <c r="J256" s="4">
+        <v>1.0900000000000001</v>
       </c>
       <c r="K256">
         <v>0.8</v>
@@ -10270,8 +10310,8 @@
       <c r="I257">
         <v>44719.62</v>
       </c>
-      <c r="J257">
-        <v>44719.62</v>
+      <c r="J257" s="2">
+        <v>1.1100000000000001</v>
       </c>
       <c r="K257">
         <v>4.0999999999999996</v>
@@ -10308,8 +10348,8 @@
       <c r="I258">
         <v>26694.92</v>
       </c>
-      <c r="J258">
-        <v>26694.92</v>
+      <c r="J258" s="4">
+        <v>0.92</v>
       </c>
       <c r="K258">
         <v>11.4</v>
@@ -10346,8 +10386,8 @@
       <c r="I259">
         <v>28457.279999999999</v>
       </c>
-      <c r="J259">
-        <v>28457.279999999999</v>
+      <c r="J259" s="2">
+        <v>0.98</v>
       </c>
       <c r="K259">
         <v>14.8</v>
@@ -10384,8 +10424,8 @@
       <c r="I260">
         <v>103240.52</v>
       </c>
-      <c r="J260">
-        <v>103240.52</v>
+      <c r="J260" s="4">
+        <v>1.32</v>
       </c>
       <c r="K260">
         <v>9.1</v>
@@ -10422,8 +10462,8 @@
       <c r="I261">
         <v>23377.34</v>
       </c>
-      <c r="J261">
-        <v>23377.34</v>
+      <c r="J261" s="2">
+        <v>0.73</v>
       </c>
       <c r="K261">
         <v>14.2</v>
@@ -10460,8 +10500,8 @@
       <c r="I262">
         <v>41619.620000000003</v>
       </c>
-      <c r="J262">
-        <v>41619.620000000003</v>
+      <c r="J262" s="4">
+        <v>1.1399999999999999</v>
       </c>
       <c r="K262">
         <v>6.4</v>
@@ -10498,8 +10538,8 @@
       <c r="I263">
         <v>89445.17</v>
       </c>
-      <c r="J263">
-        <v>89445.17</v>
+      <c r="J263" s="2">
+        <v>1.2</v>
       </c>
       <c r="K263">
         <v>2.7</v>
@@ -10536,8 +10576,8 @@
       <c r="I264">
         <v>82029.22</v>
       </c>
-      <c r="J264">
-        <v>82029.22</v>
+      <c r="J264" s="4">
+        <v>0.96</v>
       </c>
       <c r="K264">
         <v>2.1</v>
@@ -10574,8 +10614,8 @@
       <c r="I265">
         <v>28170.86</v>
       </c>
-      <c r="J265">
-        <v>28170.86</v>
+      <c r="J265" s="2">
+        <v>0.86</v>
       </c>
       <c r="K265">
         <v>8.1</v>
@@ -10612,8 +10652,8 @@
       <c r="I266">
         <v>29777.11</v>
       </c>
-      <c r="J266">
-        <v>29777.11</v>
+      <c r="J266" s="4">
+        <v>1.04</v>
       </c>
       <c r="K266">
         <v>2.5</v>
@@ -10650,8 +10690,8 @@
       <c r="I267">
         <v>19350.61</v>
       </c>
-      <c r="J267">
-        <v>19350.61</v>
+      <c r="J267" s="2">
+        <v>0.66</v>
       </c>
       <c r="K267">
         <v>10.6</v>
@@ -10688,8 +10728,8 @@
       <c r="I268">
         <v>33573.879999999997</v>
       </c>
-      <c r="J268">
-        <v>33573.879999999997</v>
+      <c r="J268" s="4">
+        <v>0.87</v>
       </c>
       <c r="K268">
         <v>6</v>
@@ -10726,8 +10766,8 @@
       <c r="I269">
         <v>25875.7</v>
       </c>
-      <c r="J269">
-        <v>25875.7</v>
+      <c r="J269" s="2">
+        <v>0.71</v>
       </c>
       <c r="K269">
         <v>7.5</v>
@@ -10764,8 +10804,8 @@
       <c r="I270">
         <v>72598.69</v>
       </c>
-      <c r="J270">
-        <v>72598.69</v>
+      <c r="J270" s="4">
+        <v>1.1000000000000001</v>
       </c>
       <c r="K270">
         <v>5.0999999999999996</v>
@@ -10802,8 +10842,8 @@
       <c r="I271">
         <v>73369.08</v>
       </c>
-      <c r="J271">
-        <v>73369.08</v>
+      <c r="J271" s="2">
+        <v>1.07</v>
       </c>
       <c r="K271">
         <v>4.2</v>
@@ -10840,8 +10880,8 @@
       <c r="I272">
         <v>77366.080000000002</v>
       </c>
-      <c r="J272">
-        <v>77366.080000000002</v>
+      <c r="J272" s="2">
+        <v>1.02</v>
       </c>
       <c r="K272">
         <v>7.7</v>
@@ -10878,8 +10918,8 @@
       <c r="I273">
         <v>21007.9</v>
       </c>
-      <c r="J273">
-        <v>21007.9</v>
+      <c r="J273" s="4">
+        <v>0.72</v>
       </c>
       <c r="K273">
         <v>11</v>
@@ -10916,8 +10956,8 @@
       <c r="I274">
         <v>36815.15</v>
       </c>
-      <c r="J274">
-        <v>36815.15</v>
+      <c r="J274" s="2">
+        <v>0.86</v>
       </c>
       <c r="K274">
         <v>7.4</v>
@@ -10954,8 +10994,8 @@
       <c r="I275">
         <v>88318.32</v>
       </c>
-      <c r="J275">
-        <v>88318.32</v>
+      <c r="J275" s="4">
+        <v>1.18</v>
       </c>
       <c r="K275">
         <v>1.9</v>
@@ -10992,8 +11032,8 @@
       <c r="I276">
         <v>82401.95</v>
       </c>
-      <c r="J276">
-        <v>82401.95</v>
+      <c r="J276" s="2">
+        <v>1.08</v>
       </c>
       <c r="K276">
         <v>6.7</v>
@@ -11030,8 +11070,8 @@
       <c r="I277">
         <v>38573.56</v>
       </c>
-      <c r="J277">
-        <v>38573.56</v>
+      <c r="J277" s="4">
+        <v>0.97</v>
       </c>
       <c r="K277">
         <v>15</v>
@@ -11068,8 +11108,8 @@
       <c r="I278">
         <v>91633.63</v>
       </c>
-      <c r="J278">
-        <v>91633.63</v>
+      <c r="J278" s="2">
+        <v>1.25</v>
       </c>
       <c r="K278">
         <v>16.7</v>
@@ -11106,8 +11146,8 @@
       <c r="I279">
         <v>39191.910000000003</v>
       </c>
-      <c r="J279">
-        <v>39191.910000000003</v>
+      <c r="J279" s="4">
+        <v>0.88</v>
       </c>
       <c r="K279">
         <v>1.8</v>
@@ -11144,8 +11184,8 @@
       <c r="I280">
         <v>48112.15</v>
       </c>
-      <c r="J280">
-        <v>48112.15</v>
+      <c r="J280" s="2">
+        <v>1.05</v>
       </c>
       <c r="K280">
         <v>6.2</v>
@@ -11182,8 +11222,8 @@
       <c r="I281">
         <v>66602.92</v>
       </c>
-      <c r="J281">
-        <v>66602.92</v>
+      <c r="J281" s="4">
+        <v>0.97</v>
       </c>
       <c r="K281">
         <v>4.2</v>
@@ -11220,8 +11260,8 @@
       <c r="I282">
         <v>26799.61</v>
       </c>
-      <c r="J282">
-        <v>26799.61</v>
+      <c r="J282" s="2">
+        <v>0.89</v>
       </c>
       <c r="K282">
         <v>14.9</v>
@@ -11258,8 +11298,8 @@
       <c r="I283">
         <v>53633.5</v>
       </c>
-      <c r="J283">
-        <v>53633.5</v>
+      <c r="J283" s="4">
+        <v>1.05</v>
       </c>
       <c r="K283">
         <v>3.8</v>
@@ -11296,8 +11336,8 @@
       <c r="I284">
         <v>47737.9</v>
       </c>
-      <c r="J284">
-        <v>47737.9</v>
+      <c r="J284" s="2">
+        <v>1.1299999999999999</v>
       </c>
       <c r="K284">
         <v>3.7</v>
@@ -11334,8 +11374,8 @@
       <c r="I285">
         <v>29236</v>
       </c>
-      <c r="J285">
-        <v>29236</v>
+      <c r="J285" s="4">
+        <v>0.95</v>
       </c>
       <c r="K285">
         <v>12.6</v>
@@ -11372,8 +11412,8 @@
       <c r="I286">
         <v>31624.83</v>
       </c>
-      <c r="J286">
-        <v>31624.83</v>
+      <c r="J286" s="2">
+        <v>0.94</v>
       </c>
       <c r="K286">
         <v>12.4</v>
@@ -11410,8 +11450,8 @@
       <c r="I287">
         <v>107137.13</v>
       </c>
-      <c r="J287">
-        <v>107137.13</v>
+      <c r="J287" s="4">
+        <v>1.3</v>
       </c>
       <c r="K287">
         <v>5.3</v>
@@ -11448,8 +11488,8 @@
       <c r="I288">
         <v>27532.43</v>
       </c>
-      <c r="J288">
-        <v>27532.43</v>
+      <c r="J288" s="2">
+        <v>0.72</v>
       </c>
       <c r="K288">
         <v>15.8</v>
@@ -11486,8 +11526,8 @@
       <c r="I289">
         <v>43340.1</v>
       </c>
-      <c r="J289">
-        <v>43340.1</v>
+      <c r="J289" s="4">
+        <v>1.1200000000000001</v>
       </c>
       <c r="K289">
         <v>1.6</v>
@@ -11524,8 +11564,8 @@
       <c r="I290">
         <v>95580.75</v>
       </c>
-      <c r="J290">
-        <v>95580.75</v>
+      <c r="J290" s="2">
+        <v>1.18</v>
       </c>
       <c r="K290">
         <v>7.9</v>
@@ -11562,8 +11602,8 @@
       <c r="I291">
         <v>86394.41</v>
       </c>
-      <c r="J291">
-        <v>86394.41</v>
+      <c r="J291" s="4">
+        <v>0.96</v>
       </c>
       <c r="K291">
         <v>8.6</v>
@@ -11600,8 +11640,8 @@
       <c r="I292">
         <v>32238.13</v>
       </c>
-      <c r="J292">
-        <v>32238.13</v>
+      <c r="J292" s="2">
+        <v>0.86</v>
       </c>
       <c r="K292">
         <v>13.9</v>
@@ -11638,8 +11678,8 @@
       <c r="I293">
         <v>32102.18</v>
       </c>
-      <c r="J293">
-        <v>32102.18</v>
+      <c r="J293" s="4">
+        <v>1.07</v>
       </c>
       <c r="K293">
         <v>7.1</v>
@@ -11676,8 +11716,8 @@
       <c r="I294">
         <v>22340.71</v>
       </c>
-      <c r="J294">
-        <v>22340.71</v>
+      <c r="J294" s="2">
+        <v>0.67</v>
       </c>
       <c r="K294">
         <v>13.3</v>
@@ -11714,8 +11754,8 @@
       <c r="I295">
         <v>36666.230000000003</v>
       </c>
-      <c r="J295">
-        <v>36666.230000000003</v>
+      <c r="J295" s="4">
+        <v>0.87</v>
       </c>
       <c r="K295">
         <v>8.1999999999999993</v>
@@ -11752,8 +11792,8 @@
       <c r="I296">
         <v>30855.119999999999</v>
       </c>
-      <c r="J296">
-        <v>30855.119999999999</v>
+      <c r="J296" s="2">
+        <v>0.71</v>
       </c>
       <c r="K296">
         <v>8.8000000000000007</v>
@@ -11790,8 +11830,8 @@
       <c r="I297">
         <v>74928.89</v>
       </c>
-      <c r="J297">
-        <v>74928.89</v>
+      <c r="J297" s="4">
+        <v>1.0900000000000001</v>
       </c>
       <c r="K297">
         <v>5</v>
@@ -11828,8 +11868,8 @@
       <c r="I298">
         <v>71184.44</v>
       </c>
-      <c r="J298">
-        <v>71184.44</v>
+      <c r="J298" s="2">
+        <v>1.08</v>
       </c>
       <c r="K298">
         <v>6.8</v>
@@ -11866,8 +11906,8 @@
       <c r="I299">
         <v>80070.38</v>
       </c>
-      <c r="J299">
-        <v>80070.38</v>
+      <c r="J299" s="7">
+        <v>1</v>
       </c>
       <c r="K299">
         <v>2.2000000000000002</v>
@@ -11904,8 +11944,8 @@
       <c r="I300">
         <v>23374.92</v>
       </c>
-      <c r="J300">
-        <v>23374.92</v>
+      <c r="J300" s="6">
+        <v>0.7</v>
       </c>
       <c r="K300">
         <v>9</v>
@@ -11942,8 +11982,8 @@
       <c r="I301">
         <v>36075.78</v>
       </c>
-      <c r="J301">
-        <v>36075.78</v>
+      <c r="J301" s="6">
+        <v>0.84</v>
       </c>
       <c r="K301">
         <v>5</v>
@@ -11980,8 +12020,8 @@
       <c r="I302">
         <v>91712.37</v>
       </c>
-      <c r="J302">
-        <v>91712.37</v>
+      <c r="J302" s="6">
+        <v>1.1599999999999999</v>
       </c>
       <c r="K302">
         <v>1.4</v>
@@ -12018,8 +12058,8 @@
       <c r="I303">
         <v>86371.97</v>
       </c>
-      <c r="J303">
-        <v>86371.97</v>
+      <c r="J303" s="6">
+        <v>1.06</v>
       </c>
       <c r="K303">
         <v>5.5</v>
@@ -12056,8 +12096,8 @@
       <c r="I304">
         <v>39965.17</v>
       </c>
-      <c r="J304">
-        <v>39965.17</v>
+      <c r="J304" s="6">
+        <v>0.95</v>
       </c>
       <c r="K304">
         <v>6.1</v>
@@ -12094,8 +12134,8 @@
       <c r="I305">
         <v>95775.59</v>
       </c>
-      <c r="J305">
-        <v>95775.59</v>
+      <c r="J305" s="6">
+        <v>1.23</v>
       </c>
       <c r="K305">
         <v>4.9000000000000004</v>
@@ -12132,8 +12172,8 @@
       <c r="I306">
         <v>41142.43</v>
       </c>
-      <c r="J306">
-        <v>41142.43</v>
+      <c r="J306" s="6">
+        <v>0.86</v>
       </c>
       <c r="K306">
         <v>5</v>
@@ -12170,8 +12210,8 @@
       <c r="I307">
         <v>50059.75</v>
       </c>
-      <c r="J307">
-        <v>50059.75</v>
+      <c r="J307" s="6">
+        <v>1.03</v>
       </c>
       <c r="K307">
         <v>4.2</v>
@@ -12208,8 +12248,8 @@
       <c r="I308">
         <v>68228.39</v>
       </c>
-      <c r="J308">
-        <v>68228.39</v>
+      <c r="J308" s="6">
+        <v>0.95</v>
       </c>
       <c r="K308">
         <v>2.4</v>
@@ -12246,8 +12286,8 @@
       <c r="I309">
         <v>29522.86</v>
       </c>
-      <c r="J309">
-        <v>29522.86</v>
+      <c r="J309" s="6">
+        <v>0.87</v>
       </c>
       <c r="K309">
         <v>13.6</v>
@@ -12284,8 +12324,8 @@
       <c r="I310">
         <v>54471.94</v>
       </c>
-      <c r="J310">
-        <v>54471.94</v>
+      <c r="J310" s="6">
+        <v>1.03</v>
       </c>
       <c r="K310">
         <v>4.2</v>
@@ -12322,8 +12362,8 @@
       <c r="I311">
         <v>49273.1</v>
       </c>
-      <c r="J311">
-        <v>49273.1</v>
+      <c r="J311" s="6">
+        <v>1.1099999999999999</v>
       </c>
       <c r="K311">
         <v>3.1</v>
@@ -12360,8 +12400,8 @@
       <c r="I312">
         <v>31500.43</v>
       </c>
-      <c r="J312">
-        <v>31500.43</v>
+      <c r="J312" s="6">
+        <v>0.92999999999999994</v>
       </c>
       <c r="K312">
         <v>8.6</v>
@@ -12398,8 +12438,8 @@
       <c r="I313">
         <v>34128.129999999997</v>
       </c>
-      <c r="J313">
-        <v>34128.129999999997</v>
+      <c r="J313" s="6">
+        <v>0.91999999999999993</v>
       </c>
       <c r="K313">
         <v>8</v>
@@ -12436,8 +12476,8 @@
       <c r="I314">
         <v>110437.78</v>
       </c>
-      <c r="J314">
-        <v>110437.78</v>
+      <c r="J314" s="6">
+        <v>1.28</v>
       </c>
       <c r="K314">
         <v>2.2000000000000002</v>
@@ -12474,8 +12514,8 @@
       <c r="I315">
         <v>29787.8</v>
       </c>
-      <c r="J315">
-        <v>29787.8</v>
+      <c r="J315" s="6">
+        <v>0.7</v>
       </c>
       <c r="K315">
         <v>11.7</v>
@@ -12512,8 +12552,8 @@
       <c r="I316">
         <v>48048.08</v>
       </c>
-      <c r="J316">
-        <v>48048.08</v>
+      <c r="J316" s="6">
+        <v>1.1000000000000001</v>
       </c>
       <c r="K316">
         <v>4.5999999999999996</v>
@@ -12550,8 +12590,8 @@
       <c r="I317">
         <v>101464.96000000001</v>
       </c>
-      <c r="J317">
-        <v>101464.96000000001</v>
+      <c r="J317" s="6">
+        <v>1.1599999999999999</v>
       </c>
       <c r="K317">
         <v>6</v>
@@ -12588,8 +12628,8 @@
       <c r="I318">
         <v>93721.82</v>
       </c>
-      <c r="J318">
-        <v>93721.82</v>
+      <c r="J318" s="6">
+        <v>0.94</v>
       </c>
       <c r="K318">
         <v>10.1</v>
@@ -12626,8 +12666,8 @@
       <c r="I319">
         <v>39119.699999999997</v>
       </c>
-      <c r="J319">
-        <v>39119.699999999997</v>
+      <c r="J319" s="6">
+        <v>0.84</v>
       </c>
       <c r="K319">
         <v>8.1</v>
@@ -12664,8 +12704,8 @@
       <c r="I320">
         <v>35393.83</v>
       </c>
-      <c r="J320">
-        <v>35393.83</v>
+      <c r="J320" s="6">
+        <v>1.05</v>
       </c>
       <c r="K320">
         <v>6.9</v>
@@ -12702,8 +12742,8 @@
       <c r="I321">
         <v>26766.05</v>
       </c>
-      <c r="J321">
-        <v>26766.05</v>
+      <c r="J321" s="6">
+        <v>0.65</v>
       </c>
       <c r="K321">
         <v>17.8</v>
@@ -12740,8 +12780,8 @@
       <c r="I322">
         <v>38208.879999999997</v>
       </c>
-      <c r="J322">
-        <v>38208.879999999997</v>
+      <c r="J322" s="6">
+        <v>0.85</v>
       </c>
       <c r="K322">
         <v>5</v>
@@ -12778,8 +12818,8 @@
       <c r="I323">
         <v>32939.72</v>
       </c>
-      <c r="J323">
-        <v>32939.72</v>
+      <c r="J323" s="6">
+        <v>0.69</v>
       </c>
       <c r="K323">
         <v>5</v>
@@ -12816,8 +12856,8 @@
       <c r="I324">
         <v>76149.87</v>
       </c>
-      <c r="J324">
-        <v>76149.87</v>
+      <c r="J324" s="6">
+        <v>1.07</v>
       </c>
       <c r="K324">
         <v>-0.1</v>
@@ -12854,8 +12894,8 @@
       <c r="I325">
         <v>75075.600000000006</v>
       </c>
-      <c r="J325">
-        <v>75075.600000000006</v>
+      <c r="J325" s="6">
+        <v>1.06</v>
       </c>
       <c r="K325">
         <v>3.3</v>

</xml_diff>